<commit_message>
Updated Members List and Footer
</commit_message>
<xml_diff>
--- a/public/Members.xlsx
+++ b/public/Members.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelsong/Documents/GitHub/hackduke.org/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EED8B1-9BE8-1841-A5DC-1D9DF82907D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C6D6E0-8B2E-D642-BBB5-81A2CEF0BCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15920" yWindow="1620" windowWidth="14320" windowHeight="16340" xr2:uid="{A8C4F12F-2955-4C9C-BF55-E94716F42DC1}"/>
+    <workbookView xWindow="4040" yWindow="1620" windowWidth="26200" windowHeight="16340" xr2:uid="{A8C4F12F-2955-4C9C-BF55-E94716F42DC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="148">
   <si>
     <t>Team</t>
   </si>
@@ -442,9 +442,6 @@
     <t>https://www.linkedin.com/in/christianokokhere/</t>
   </si>
   <si>
-    <t>CS, Neuroscience &amp; Econ</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/isabelle-xiong-368257204</t>
   </si>
   <si>
@@ -466,23 +463,40 @@
     <t>https://www.linkedin.com/in/caoandrew/</t>
   </si>
   <si>
-    <t>Bio</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/debi-ahitov</t>
   </si>
   <si>
     <t>https://www.linkedin.com/in/mariam-gvenetadze</t>
+  </si>
+  <si>
+    <t>Treasury</t>
+  </si>
+  <si>
+    <t>Bio &amp; CS</t>
+  </si>
+  <si>
+    <t>Math &amp; CS</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/amy-heqing-yin-b20a73251/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -505,13 +519,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -826,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8998A0-F69B-4662-8CC4-D03EC49F9EEE}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="118" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -862,45 +879,42 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>123</v>
       </c>
       <c r="G2">
-        <v>2024</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="G3">
         <v>2025</v>
@@ -908,68 +922,68 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>126</v>
       </c>
       <c r="G4">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
       <c r="G5">
-        <v>2024</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="G6">
         <v>2026</v>
@@ -977,22 +991,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>127</v>
       </c>
       <c r="G7">
         <v>2025</v>
@@ -1000,180 +1014,180 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="G8">
-        <v>2026</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s">
         <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G9">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>109</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="G10">
-        <v>2025</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>110</v>
+        <v>24</v>
       </c>
       <c r="G11">
-        <v>2024</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="G12">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>109</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G13">
-        <v>2024</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>114</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G14">
-        <v>2024</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
         <v>63</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
       <c r="F15" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="G15">
         <v>2025</v>
@@ -1181,33 +1195,33 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
         <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F16" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G16">
-        <v>2026</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
         <v>63</v>
@@ -1216,21 +1230,21 @@
         <v>28</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="G17">
-        <v>2024</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
         <v>63</v>
@@ -1239,79 +1253,79 @@
         <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>118</v>
+        <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G18">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
         <v>21</v>
       </c>
       <c r="F19" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="G19">
-        <v>2023</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" t="s">
-        <v>121</v>
+        <v>146</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="G20">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="D21" t="s">
         <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>145</v>
       </c>
       <c r="F21" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="G21">
         <v>2026</v>
@@ -1319,36 +1333,30 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" t="s">
-        <v>123</v>
+        <v>28</v>
       </c>
       <c r="G22">
-        <v>2025</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
         <v>16</v>
@@ -1356,65 +1364,68 @@
       <c r="E23" t="s">
         <v>34</v>
       </c>
+      <c r="F23" t="s">
+        <v>110</v>
+      </c>
       <c r="G23">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E24" t="s">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="F24" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="G24">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
       </c>
       <c r="E25" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="F25" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="G25">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1422,97 +1433,100 @@
       <c r="E26" t="s">
         <v>34</v>
       </c>
+      <c r="F26" t="s">
+        <v>111</v>
+      </c>
       <c r="G26">
         <v>2025</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="D27" t="s">
         <v>28</v>
       </c>
       <c r="E27" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F27" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="G27">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E28" t="s">
         <v>34</v>
       </c>
       <c r="F28" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="G28">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E29" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F29" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G29">
-        <v>2024</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D30" t="s">
         <v>28</v>
       </c>
       <c r="E30" t="s">
-        <v>34</v>
+        <v>137</v>
       </c>
       <c r="F30" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="G30">
         <v>2026</v>
@@ -1520,22 +1534,16 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
         <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" t="s">
-        <v>132</v>
-      </c>
-      <c r="F31" t="s">
-        <v>133</v>
+        <v>28</v>
       </c>
       <c r="G31">
         <v>2025</v>
@@ -1543,33 +1551,30 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C32" t="s">
         <v>83</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E32" t="s">
         <v>34</v>
       </c>
-      <c r="F32" t="s">
-        <v>134</v>
-      </c>
       <c r="G32">
         <v>2025</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C33" t="s">
         <v>83</v>
@@ -1578,21 +1583,21 @@
         <v>28</v>
       </c>
       <c r="E33" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F33" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G33">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C34" t="s">
         <v>83</v>
@@ -1600,22 +1605,16 @@
       <c r="D34" t="s">
         <v>28</v>
       </c>
-      <c r="E34" t="s">
-        <v>138</v>
-      </c>
-      <c r="F34" t="s">
-        <v>137</v>
-      </c>
       <c r="G34">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C35" t="s">
         <v>83</v>
@@ -1623,16 +1622,22 @@
       <c r="D35" t="s">
         <v>28</v>
       </c>
+      <c r="E35" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" t="s">
+        <v>135</v>
+      </c>
       <c r="G35">
         <v>2025</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C36" t="s">
         <v>83</v>
@@ -1641,7 +1646,10 @@
         <v>28</v>
       </c>
       <c r="E36" t="s">
-        <v>34</v>
+        <v>140</v>
+      </c>
+      <c r="F36" t="s">
+        <v>139</v>
       </c>
       <c r="G36">
         <v>2025</v>
@@ -1649,22 +1657,22 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E37" t="s">
-        <v>132</v>
+        <v>21</v>
       </c>
       <c r="F37" t="s">
-        <v>139</v>
+        <v>22</v>
       </c>
       <c r="G37">
         <v>2024</v>
@@ -1672,79 +1680,88 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="D38" t="s">
-        <v>28</v>
+        <v>16</v>
+      </c>
+      <c r="E38" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" t="s">
+        <v>23</v>
       </c>
       <c r="G38">
-        <v>2025</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="D39" t="s">
         <v>28</v>
       </c>
       <c r="E39" t="s">
-        <v>141</v>
+        <v>20</v>
       </c>
       <c r="F39" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="G39">
-        <v>2025</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="D40" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E40" t="s">
-        <v>21</v>
-      </c>
-      <c r="F40" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="G40">
-        <v>2025</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>16</v>
+        <v>28</v>
+      </c>
+      <c r="E41" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" t="s">
+        <v>33</v>
       </c>
       <c r="G41">
         <v>2025</v>
@@ -1752,22 +1769,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="D42" t="s">
         <v>28</v>
       </c>
       <c r="E42" t="s">
-        <v>143</v>
+        <v>34</v>
       </c>
       <c r="F42" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="G42">
         <v>2026</v>
@@ -1775,16 +1792,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="D43" t="s">
         <v>28</v>
+      </c>
+      <c r="E43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" t="s">
+        <v>30</v>
       </c>
       <c r="G43">
         <v>2026</v>
@@ -1798,7 +1821,7 @@
         <v>105</v>
       </c>
       <c r="C44" t="s">
-        <v>2</v>
+        <v>144</v>
       </c>
       <c r="D44" t="s">
         <v>106</v>
@@ -1807,13 +1830,22 @@
         <v>34</v>
       </c>
       <c r="F44" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G44">
         <v>2025</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G44">
+    <sortCondition ref="C2:C44"/>
+    <sortCondition ref="D2:D44"/>
+    <sortCondition ref="B2:B44"/>
+    <sortCondition ref="A2:A44"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="F20" r:id="rId1" xr:uid="{B67C3C2A-B7CF-3E42-B00E-72ED7150005F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>